<commit_message>
Second commit for Selenium
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/testdata.xlsx
+++ b/src/test/resources/testdata/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eclipse-workspace\SeleniumAutomationFramework\TestAutomationFramework\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD575E4A-DB51-4076-80E0-8E9CF1B40D9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28CF2BF5-F8A2-437C-BEC3-79E9FD70CFE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="loginTest" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="9">
   <si>
     <t>username</t>
   </si>
@@ -43,78 +43,6 @@
     <t>password</t>
   </si>
   <si>
-    <t>sohail2021@gmail.com</t>
-  </si>
-  <si>
-    <t>Auto@24</t>
-  </si>
-  <si>
-    <t>sheikh2021@gmail.com</t>
-  </si>
-  <si>
-    <t>sheikhsohail@gmail.com</t>
-  </si>
-  <si>
-    <t>sheikhsohail2021@gmail.com</t>
-  </si>
-  <si>
-    <t>Auto@proj24</t>
-  </si>
-  <si>
-    <t>Autoproj24</t>
-  </si>
-  <si>
-    <t>proj24</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>xy</t>
-  </si>
-  <si>
-    <t>xyz</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>ab</t>
-  </si>
-  <si>
-    <t>abc</t>
-  </si>
-  <si>
-    <t>first</t>
-  </si>
-  <si>
-    <t>second</t>
-  </si>
-  <si>
-    <t>third</t>
-  </si>
-  <si>
-    <t>xa</t>
-  </si>
-  <si>
-    <t>xyzabc</t>
-  </si>
-  <si>
-    <t>xyab</t>
-  </si>
-  <si>
-    <t>fourth</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>f</t>
-  </si>
-  <si>
     <t>wrong_username</t>
   </si>
   <si>
@@ -125,24 +53,25 @@
   </si>
   <si>
     <t>correct_password</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>failed</t>
+  </si>
+  <si>
+    <t>passed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -165,16 +94,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -455,8 +381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -475,34 +401,34 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -513,120 +439,74 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B9C9E1B-D3BE-4CEA-8A72-4C01801D8670}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17.5546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A6" r:id="rId1" xr:uid="{7F87E3D5-0EC3-4A8B-A17F-8D4B157A95DA}"/>
-    <hyperlink ref="B6" r:id="rId2" display="Auto@24" xr:uid="{62824F59-8B7B-4ACA-8C23-45ED6827EC7C}"/>
-    <hyperlink ref="A7" r:id="rId3" xr:uid="{0887D6AA-4A29-420B-B739-F725DF9F7ACA}"/>
-    <hyperlink ref="A8" r:id="rId4" xr:uid="{5D53B2AC-53E8-4861-9C8B-7BAE71F8078D}"/>
-    <hyperlink ref="A9" r:id="rId5" xr:uid="{AD6D5462-BADA-4796-BF56-BC1C04030489}"/>
-    <hyperlink ref="B9" r:id="rId6" xr:uid="{95DFB31B-AB63-4FE0-8FDD-79C7A7B793EA}"/>
-    <hyperlink ref="B7" r:id="rId7" xr:uid="{2F046010-3038-4D0B-9AC5-F076D621E393}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Second commit for Selenium Java automation code
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/testdata.xlsx
+++ b/src/test/resources/testdata/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eclipse-workspace\SeleniumAutomationFramework\TestAutomationFramework\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28CF2BF5-F8A2-437C-BEC3-79E9FD70CFE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C9C7CDD-02C3-4233-AC47-C67519D690EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="11">
   <si>
     <t>username</t>
   </si>
@@ -55,13 +55,19 @@
     <t>correct_password</t>
   </si>
   <si>
-    <t>status</t>
-  </si>
-  <si>
     <t>failed</t>
   </si>
   <si>
     <t>passed</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Status</t>
   </si>
 </sst>
 </file>
@@ -442,7 +448,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -453,13 +459,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -470,7 +476,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -481,7 +487,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -492,7 +498,7 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -503,7 +509,7 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>